<commit_message>
add note 1, not finished yet
</commit_message>
<xml_diff>
--- a/资源/笔记/Golang讲解的示意图.xlsx
+++ b/资源/笔记/Golang讲解的示意图.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22228"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B21E936E-C3F4-41AA-B8C4-00E62660CB28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +17,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -65,6 +66,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -81,7 +85,13 @@
     <xdr:ext cx="4698722" cy="359073"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -138,7 +148,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="圆角矩形 2"/>
+        <xdr:cNvPr id="3" name="圆角矩形 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -193,7 +209,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
-            <a:t>页面布局刷新问题</a:t>
+            <a:t>页面局部刷新问题</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
@@ -230,7 +246,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="右箭头 3"/>
+        <xdr:cNvPr id="4" name="右箭头 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -284,7 +306,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="圆角矩形 4"/>
+        <xdr:cNvPr id="5" name="圆角矩形 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -389,7 +417,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="右箭头 5"/>
+        <xdr:cNvPr id="6" name="右箭头 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -443,7 +477,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="圆角矩形 6"/>
+        <xdr:cNvPr id="7" name="圆角矩形 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -524,7 +564,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="右箭头 7"/>
+        <xdr:cNvPr id="8" name="右箭头 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -578,7 +624,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="圆角矩形 8"/>
+        <xdr:cNvPr id="9" name="圆角矩形 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -676,7 +728,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="右箭头 9"/>
+        <xdr:cNvPr id="10" name="右箭头 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -730,7 +788,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="圆角矩形 10"/>
+        <xdr:cNvPr id="11" name="圆角矩形 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -934,7 +998,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="13" name="直接箭头连接符 12"/>
+        <xdr:cNvPr id="13" name="直接箭头连接符 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="11" idx="1"/>
         </xdr:cNvCxnSpPr>
@@ -983,7 +1053,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="15" name="直接连接符 14"/>
+        <xdr:cNvPr id="15" name="直接连接符 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -1027,7 +1103,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="16" name="直接连接符 15"/>
+        <xdr:cNvPr id="16" name="直接连接符 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000010000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -1071,7 +1153,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="19" name="直接连接符 18"/>
+        <xdr:cNvPr id="19" name="直接连接符 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000013000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -1115,7 +1203,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="20" name="笑脸 19"/>
+        <xdr:cNvPr id="20" name="笑脸 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000014000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1172,7 +1266,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="21" name="笑脸 20"/>
+        <xdr:cNvPr id="21" name="笑脸 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000015000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1229,7 +1329,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="22" name="右箭头 21"/>
+        <xdr:cNvPr id="22" name="右箭头 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000016000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1281,7 +1387,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="23" name="TextBox 22"/>
+        <xdr:cNvPr id="23" name="TextBox 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000017000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1384,7 +1496,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="24" name="圆角矩形 23"/>
+        <xdr:cNvPr id="24" name="圆角矩形 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1468,7 +1586,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="29" name="笑脸 28"/>
+        <xdr:cNvPr id="29" name="笑脸 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1525,7 +1649,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="30" name="右箭头 29"/>
+        <xdr:cNvPr id="30" name="右箭头 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1577,7 +1707,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="31" name="TextBox 30"/>
+        <xdr:cNvPr id="31" name="TextBox 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1768,7 +1904,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="32" name="TextBox 31"/>
+        <xdr:cNvPr id="32" name="TextBox 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000020000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1853,7 +1995,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name="圆角矩形 11"/>
+        <xdr:cNvPr id="12" name="圆角矩形 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1941,7 +2089,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="14" name="TextBox 13"/>
+        <xdr:cNvPr id="14" name="TextBox 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2024,7 +2178,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="17" name="右箭头 16"/>
+        <xdr:cNvPr id="17" name="右箭头 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000011000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2076,7 +2236,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="28" name="圆角矩形 27"/>
+        <xdr:cNvPr id="28" name="圆角矩形 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2144,7 +2310,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="33" name="右箭头 32"/>
+        <xdr:cNvPr id="33" name="右箭头 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000021000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2196,7 +2368,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="18" name="TextBox 17"/>
+        <xdr:cNvPr id="18" name="TextBox 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000012000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2293,7 +2471,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="25" name="右箭头 24"/>
+        <xdr:cNvPr id="25" name="右箭头 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000019000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2347,7 +2531,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="26" name="TextBox 25"/>
+        <xdr:cNvPr id="26" name="TextBox 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2456,7 +2646,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="27" name="TextBox 26"/>
+        <xdr:cNvPr id="27" name="TextBox 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2547,7 +2743,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="34" name="图片 33"/>
+        <xdr:cNvPr id="34" name="图片 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000022000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2585,7 +2787,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="35" name="图片 34"/>
+        <xdr:cNvPr id="35" name="图片 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2623,7 +2831,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="36" name="左右箭头 35"/>
+        <xdr:cNvPr id="36" name="左右箭头 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000024000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2675,7 +2889,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="37" name="图片 36"/>
+        <xdr:cNvPr id="37" name="图片 36">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000025000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2713,7 +2933,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="39" name="直接箭头连接符 38"/>
+        <xdr:cNvPr id="39" name="直接箭头连接符 38">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000027000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -2755,7 +2981,13 @@
     <xdr:ext cx="387607" cy="264560"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="40" name="TextBox 39"/>
+        <xdr:cNvPr id="40" name="TextBox 39">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000028000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2813,7 +3045,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="41" name="图片 40"/>
+        <xdr:cNvPr id="41" name="图片 40">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000029000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2851,7 +3089,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="43" name="直接箭头连接符 42"/>
+        <xdr:cNvPr id="43" name="直接箭头连接符 42">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -2893,7 +3137,13 @@
     <xdr:ext cx="2281330" cy="998094"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="44" name="TextBox 43"/>
+        <xdr:cNvPr id="44" name="TextBox 43">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -3027,7 +3277,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="38" name="图片 37"/>
+        <xdr:cNvPr id="38" name="图片 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000026000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3065,7 +3321,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="45" name="直接箭头连接符 44"/>
+        <xdr:cNvPr id="45" name="直接箭头连接符 44">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -3112,7 +3374,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="46" name="圆角矩形 45"/>
+        <xdr:cNvPr id="46" name="圆角矩形 45">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -3169,7 +3437,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="48" name="直接箭头连接符 47"/>
+        <xdr:cNvPr id="48" name="直接箭头连接符 47">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000030000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="38" idx="3"/>
         </xdr:cNvCxnSpPr>
@@ -3213,7 +3487,13 @@
     <xdr:ext cx="466794" cy="275717"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="49" name="TextBox 48"/>
+        <xdr:cNvPr id="49" name="TextBox 48">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000031000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -3270,7 +3550,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="50" name="圆角矩形 49"/>
+        <xdr:cNvPr id="50" name="圆角矩形 49">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000032000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -3321,7 +3607,13 @@
     <xdr:ext cx="217047" cy="264560"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="51" name="TextBox 50"/>
+        <xdr:cNvPr id="51" name="TextBox 50">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000033000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -3379,7 +3671,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="53" name="直接箭头连接符 52"/>
+        <xdr:cNvPr id="53" name="直接箭头连接符 52">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000035000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:endCxn id="50" idx="1"/>
         </xdr:cNvCxnSpPr>
@@ -3428,7 +3726,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="54" name="TextBox 53"/>
+        <xdr:cNvPr id="54" name="TextBox 53">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000036000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -3540,7 +3844,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="55" name="TextBox 54"/>
+        <xdr:cNvPr id="55" name="TextBox 54">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000037000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -3701,7 +4011,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="57" name="圆角矩形 56"/>
+        <xdr:cNvPr id="57" name="圆角矩形 56">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000039000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -3751,7 +4067,13 @@
     <xdr:ext cx="217047" cy="264560"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="58" name="TextBox 57"/>
+        <xdr:cNvPr id="58" name="TextBox 57">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -3809,7 +4131,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="59" name="圆角矩形 58"/>
+        <xdr:cNvPr id="59" name="圆角矩形 58">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -3865,7 +4193,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="61" name="直接箭头连接符 60"/>
+        <xdr:cNvPr id="61" name="直接箭头连接符 60">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="58" idx="3"/>
           <a:endCxn id="59" idx="1"/>
@@ -3910,7 +4244,13 @@
     <xdr:ext cx="1050929" cy="264560"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="62" name="TextBox 61"/>
+        <xdr:cNvPr id="62" name="TextBox 61">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -3968,7 +4308,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="66" name="图片 65"/>
+        <xdr:cNvPr id="66" name="图片 65">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000042000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -4001,7 +4347,13 @@
     <xdr:ext cx="355225" cy="264560"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="67" name="TextBox 66"/>
+        <xdr:cNvPr id="67" name="TextBox 66">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000043000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -4059,7 +4411,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="68" name="圆角矩形 67"/>
+        <xdr:cNvPr id="68" name="圆角矩形 67">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000044000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -4147,7 +4505,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="70" name="直接箭头连接符 69"/>
+        <xdr:cNvPr id="70" name="直接箭头连接符 69">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000046000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="67" idx="3"/>
           <a:endCxn id="68" idx="1"/>
@@ -4197,7 +4561,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="73" name="直接箭头连接符 72"/>
+        <xdr:cNvPr id="73" name="直接箭头连接符 72">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000049000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:endCxn id="59" idx="2"/>
         </xdr:cNvCxnSpPr>
@@ -4241,7 +4611,13 @@
     <xdr:ext cx="1008481" cy="264560"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="74" name="TextBox 73"/>
+        <xdr:cNvPr id="74" name="TextBox 73">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -4299,7 +4675,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="75" name="圆角矩形 74"/>
+        <xdr:cNvPr id="75" name="圆角矩形 74">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -4351,7 +4733,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="76" name="图片 75"/>
+        <xdr:cNvPr id="76" name="图片 75">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -4384,7 +4772,13 @@
     <xdr:ext cx="445571" cy="264560"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="77" name="TextBox 76"/>
+        <xdr:cNvPr id="77" name="TextBox 76">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -4442,7 +4836,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="78" name="圆角矩形 77"/>
+        <xdr:cNvPr id="78" name="圆角矩形 77">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -4498,7 +4898,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="80" name="直接箭头连接符 79"/>
+        <xdr:cNvPr id="80" name="直接箭头连接符 79">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000050000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="77" idx="3"/>
           <a:endCxn id="78" idx="1"/>
@@ -4548,7 +4954,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="82" name="直接箭头连接符 81"/>
+        <xdr:cNvPr id="82" name="直接箭头连接符 81">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000052000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -4590,7 +5002,13 @@
     <xdr:ext cx="355225" cy="264560"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="83" name="TextBox 82"/>
+        <xdr:cNvPr id="83" name="TextBox 82">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000053000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -4648,7 +5066,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="84" name="圆角矩形 83"/>
+        <xdr:cNvPr id="84" name="圆角矩形 83">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000054000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -4701,7 +5125,13 @@
     <xdr:ext cx="1020344" cy="264560"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="85" name="TextBox 84"/>
+        <xdr:cNvPr id="85" name="TextBox 84">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000055000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -4759,7 +5189,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="87" name="直接箭头连接符 86"/>
+        <xdr:cNvPr id="87" name="直接箭头连接符 86">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000057000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="84" idx="0"/>
         </xdr:cNvCxnSpPr>
@@ -4808,7 +5244,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="89" name="直接箭头连接符 88"/>
+        <xdr:cNvPr id="89" name="直接箭头连接符 88">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000059000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -4855,7 +5297,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="42" name="圆角矩形 41"/>
+        <xdr:cNvPr id="42" name="圆角矩形 41">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -4910,7 +5358,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="47" name="圆角矩形 46"/>
+        <xdr:cNvPr id="47" name="圆角矩形 46">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -4981,7 +5435,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="79" name="圆角矩形 78"/>
+        <xdr:cNvPr id="79" name="圆角矩形 78">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -5061,7 +5521,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="52" name="TextBox 51"/>
+        <xdr:cNvPr id="52" name="TextBox 51">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000034000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -6003,7 +6469,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -6036,9 +6502,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -6071,6 +6554,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -6246,14 +6746,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B271" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L297" sqref="L297"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6263,12 +6763,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6276,12 +6776,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>